<commit_message>
Add rate and provenance
</commit_message>
<xml_diff>
--- a/atomica/library/sir_framework.xlsx
+++ b/atomica/library/sir_framework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FBB84E-2429-4F68-B27C-D0A8149FC406}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B562A85-05B6-44B5-AE90-8DBF8AFCE4C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4545" yWindow="1815" windowWidth="23715" windowHeight="18525" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,12 @@
     <sheet name="Parameters" sheetId="6" r:id="rId6"/>
     <sheet name="Cascades" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -550,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -769,6 +770,9 @@
   </si>
   <si>
     <t>inf,rec</t>
+  </si>
+  <si>
+    <t>Rate</t>
   </si>
 </sst>
 </file>
@@ -1682,18 +1686,18 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="96.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1794,7 +1798,7 @@
         <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -1816,7 +1820,7 @@
         <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -1838,7 +1842,7 @@
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>

</xml_diff>